<commit_message>
still trobleshooting flask to html connect
</commit_message>
<xml_diff>
--- a/templates/Python/full-stack-challenge(Python).xlsx
+++ b/templates/Python/full-stack-challenge(Python).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="12" r:id="rId1"/>
@@ -2750,7 +2750,7 @@
   <dimension ref="A1:F204"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
start file i/o task
</commit_message>
<xml_diff>
--- a/templates/Python/full-stack-challenge(Python).xlsx
+++ b/templates/Python/full-stack-challenge(Python).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Full-Stack-Dev.-Challenge\templates\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\on-going-projects\Full-Stack-Dev.-Challenge\templates\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="379">
   <si>
     <t>Category</t>
   </si>
@@ -479,9 +479,6 @@
     <t>5. Build a Python debugger with advanced features like time-travel debugging and memory analysis.</t>
   </si>
   <si>
-    <t>1. Design a function decorator that enforces a specific execution order for functions.</t>
-  </si>
-  <si>
     <t>2. Implement a function cache with sophisticated cache eviction policies and memoization strategies.</t>
   </si>
   <si>
@@ -627,9 +624,6 @@
   </si>
   <si>
     <t>String Manipulation</t>
-  </si>
-  <si>
-    <t>1. Implement a high-performance string matching algorithm for pattern search in large text corpora.</t>
   </si>
   <si>
     <t>2. Design a distributed string manipulation system for processing text data across multiple nodes.</t>
@@ -1692,7 +1686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7:S11"/>
     </sheetView>
   </sheetViews>
@@ -2749,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2777,13 +2771,13 @@
         <v>137</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>138</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2815,378 +2809,374 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>143</v>
-      </c>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
       <c r="B37" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>193</v>
-      </c>
+      <c r="C47" s="9"/>
     </row>
     <row r="48" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="8"/>
       <c r="B52" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="8"/>
       <c r="B53" s="8"/>
       <c r="C53" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="8"/>
       <c r="B54" s="8"/>
       <c r="C54" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
       <c r="B55" s="8"/>
       <c r="C55" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3195,146 +3185,146 @@
         <v>4</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
       <c r="C64" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
       <c r="C66" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
       <c r="B68" s="8"/>
       <c r="C68" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="8"/>
       <c r="B74" s="8"/>
       <c r="C74" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="8"/>
       <c r="B76" s="8"/>
       <c r="C76" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3343,35 +3333,35 @@
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3380,72 +3370,72 @@
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="8"/>
       <c r="B84" s="8"/>
       <c r="C84" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="8"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
       <c r="C89" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
       <c r="B90" s="8"/>
       <c r="C90" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3454,109 +3444,109 @@
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8"/>
       <c r="B98" s="8"/>
       <c r="C98" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="8"/>
       <c r="B100" s="8"/>
       <c r="C100" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="8"/>
       <c r="B101" s="8"/>
       <c r="C101" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="8"/>
       <c r="B104" s="8"/>
       <c r="C104" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="8"/>
       <c r="B106" s="8"/>
       <c r="C106" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3565,730 +3555,730 @@
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="C108" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="8"/>
       <c r="B110" s="8"/>
       <c r="C110" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="8"/>
       <c r="B114" s="8"/>
       <c r="C114" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="8"/>
       <c r="B115" s="8"/>
       <c r="C115" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C120" s="9" t="s">
         <v>275</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C120" s="9" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="8"/>
       <c r="B121" s="8"/>
       <c r="C121" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="8"/>
       <c r="B125" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="8"/>
       <c r="B126" s="8"/>
       <c r="C126" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="8"/>
       <c r="B127" s="8"/>
       <c r="C127" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="8"/>
       <c r="B128" s="8"/>
       <c r="C128" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="8"/>
       <c r="B129" s="8"/>
       <c r="C129" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="8"/>
       <c r="B130" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="8"/>
       <c r="B131" s="8"/>
       <c r="C131" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="8"/>
       <c r="B132" s="8"/>
       <c r="C132" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="8"/>
       <c r="B133" s="8"/>
       <c r="C133" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="8"/>
       <c r="B134" s="8"/>
       <c r="C134" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="8"/>
       <c r="B135" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="8"/>
       <c r="B137" s="8"/>
       <c r="C137" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="8"/>
       <c r="B139" s="8"/>
       <c r="C139" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="8"/>
       <c r="B140" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="8"/>
       <c r="B141" s="8"/>
       <c r="C141" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="C145" s="9" t="s">
         <v>306</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="C145" s="9" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="8"/>
       <c r="B147" s="8"/>
       <c r="C147" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="8"/>
       <c r="B150" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="8"/>
       <c r="B151" s="8"/>
       <c r="C151" s="9" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="8"/>
       <c r="B152" s="8"/>
       <c r="C152" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="8"/>
       <c r="B153" s="8"/>
       <c r="C153" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="8"/>
       <c r="B155" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="8"/>
       <c r="B158" s="8"/>
       <c r="C158" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="8"/>
       <c r="B159" s="8"/>
       <c r="C159" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="8"/>
       <c r="B160" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="8"/>
       <c r="B161" s="8"/>
       <c r="C161" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="8"/>
       <c r="B163" s="8"/>
       <c r="C163" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="8"/>
       <c r="B164" s="8"/>
       <c r="C164" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="8"/>
       <c r="B165" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="8"/>
       <c r="B166" s="8"/>
       <c r="C166" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="8"/>
       <c r="B167" s="8"/>
       <c r="C167" s="9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="8"/>
       <c r="B168" s="8"/>
       <c r="C168" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="8"/>
       <c r="B169" s="8"/>
       <c r="C169" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="8"/>
       <c r="B170" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="8"/>
       <c r="B171" s="8"/>
       <c r="C171" s="9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="8"/>
       <c r="B172" s="8"/>
       <c r="C172" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="8"/>
       <c r="B173" s="8"/>
       <c r="C173" s="9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="8"/>
       <c r="B174" s="8"/>
       <c r="C174" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A175" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="8"/>
       <c r="B176" s="8"/>
       <c r="C176" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="8"/>
       <c r="B177" s="8"/>
       <c r="C177" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="C178" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="8"/>
       <c r="B179" s="8"/>
       <c r="C179" s="9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="8"/>
       <c r="B180" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="8"/>
       <c r="B181" s="8"/>
       <c r="C181" s="9" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="C182" s="9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="C183" s="9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="C184" s="9" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="8"/>
       <c r="B185" s="8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="C186" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="C187" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="C188" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
       <c r="C189" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="8"/>
       <c r="B190" s="8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="8"/>
       <c r="B191" s="8"/>
       <c r="C191" s="9" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A192" s="8"/>
       <c r="B192" s="8"/>
       <c r="C192" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
       <c r="C193" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="C194" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A195" s="8"/>
       <c r="B195" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
       <c r="C196" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="8"/>
       <c r="B197" s="8"/>
       <c r="C197" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A198" s="8"/>
       <c r="B198" s="8"/>
       <c r="C198" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
       <c r="C199" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A200" s="8"/>
       <c r="B200" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A201" s="8"/>
       <c r="B201" s="8"/>
       <c r="C201" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="C202" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="8"/>
       <c r="B203" s="8"/>
       <c r="C203" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A204" s="8"/>
       <c r="B204" s="8"/>
       <c r="C204" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add django project to collecet processed data from python script, filter, aggregate and render to html via js fetch api
</commit_message>
<xml_diff>
--- a/templates/Python/full-stack-challenge(Python).xlsx
+++ b/templates/Python/full-stack-challenge(Python).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\on-going-projects\Full-Stack-Dev.-Challenge\templates\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\on-going-projects\Full-Stack-Dev.-Challenge\templates\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7932" windowHeight="8448" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="12" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="382">
   <si>
     <t>Category</t>
   </si>
@@ -926,9 +926,6 @@
     <t>5. Build a distributed Bayesian analysis framework for probabilistic modeling and inference in large datasets.</t>
   </si>
   <si>
-    <t>Data Visualization Techniques</t>
-  </si>
-  <si>
     <t>1. Implement a distributed data visualization framework for creating interactive visualizations of large datasets.</t>
   </si>
   <si>
@@ -1181,11 +1178,26 @@
     <t>5. Build a distributed model explainability tool for interpreting and explaining the predictions of deployed machine learning models.</t>
   </si>
   <si>
-    <t>Core Python (Class 1):
+    <t>Syntax (variables, data types, operators, control flow)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Python (Class 1):
 Functions (defining, calling, arguments, return values)
 Object-Oriented Programming (classes, objects, inheritance, polymorphism)
 Modules and Packages (code organization, importing code)
-Data Structures (Class 2):
+</t>
+  </si>
+  <si>
+    <t>Advanced Topics (Class 13):
+Parallel and Distributed Computing: (using multiple processors/computers for large tasks) (Libraries: Dask, Ray)
+Scientific Computing: (numerical simulations, data analysis, scientific visualization) (Libraries: SciPy, SymPy)
+Web Scraping: (automated data extraction from websites) (Libraries: Beautiful Soup, Scrapy)
+Network Programming: (building servers, clients, network automation tools) (Libraries: socket, asyncio)
+Game Development: (creating games with frameworks like Pygame and Arcade)
+Metaheuristics and Optimization: (solving complex problems with optimization algorithms) (Libraries: SciPy, DEAP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Structures (Class 2):
 Lists (ordered collections of items)
 Tuples (immutable ordered collections)
 Sets (unordered collections of unique elements)
@@ -1241,22 +1253,17 @@
 Natural Language Processing (analyzing and generating human language)
 Computer Vision (processing and analyzing visual data)
 Model Deployment (deploying models to production)
-Data Science (Class 12):
+</t>
+  </si>
+  <si>
+    <t>Data Science (Class 12):
 Data Preprocessing (cleaning, transformation, feature engineering)
 Exploratory Data Analysis (EDA) (understanding data characteristics)
 Statistical Analysis (descriptive statistics, hypothesis testing)
-Data Visualization Techniques (creating informative charts and graphs)
-Time Series Analysis (analyzing sequential data)
-Advanced Topics (Class 13):
-Parallel and Distributed Computing: (using multiple processors/computers for large tasks) (Libraries: Dask, Ray)
-Scientific Computing: (numerical simulations, data analysis, scientific visualization) (Libraries: SciPy, SymPy)
-Web Scraping: (automated data extraction from websites) (Libraries: Beautiful Soup, Scrapy)
-Network Programming: (building servers, clients, network automation tools) (Libraries: socket, asyncio)
-Game Development: (creating games with frameworks like Pygame and Arcade)
-Metaheuristics and Optimization: (solving complex problems with optimization algorithms) (Libraries: SciPy, DEAP)</t>
-  </si>
-  <si>
-    <t>Syntax (variables, data types, operators, control flow)</t>
+Time Series Analysis (analyzing sequential data)</t>
+  </si>
+  <si>
+    <t>Data Visualization Techniques (creating informative charts and graphs)</t>
   </si>
 </sst>
 </file>
@@ -1686,7 +1693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7:S11"/>
     </sheetView>
   </sheetViews>
@@ -2743,8 +2750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C135" sqref="B135:C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2766,12 +2773,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>137</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>138</v>
@@ -2881,7 +2888,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
         <v>153</v>
@@ -2890,35 +2897,35 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>159</v>
       </c>
@@ -2928,36 +2935,39 @@
       <c r="C22" s="9" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="10" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="8" t="s">
         <v>166</v>
@@ -2966,35 +2976,35 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="8" t="s">
         <v>172</v>
@@ -3595,35 +3605,35 @@
         <v>264</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="9" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="8"/>
       <c r="B114" s="8"/>
       <c r="C114" s="9" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="8"/>
       <c r="B115" s="8"/>
       <c r="C115" s="9" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="8"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="8" t="s">
         <v>269</v>
       </c>
@@ -3632,21 +3642,21 @@
         <v>270</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="C118" s="9" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="9" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
         <v>273</v>
       </c>
@@ -3656,36 +3666,39 @@
       <c r="C120" s="9" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D120" s="10" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="8"/>
       <c r="B121" s="8"/>
       <c r="C121" s="9" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="C122" s="9" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="9" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="C124" s="9" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="8"/>
       <c r="B125" s="8" t="s">
         <v>280</v>
@@ -3694,21 +3707,21 @@
         <v>281</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="8"/>
       <c r="B126" s="8"/>
       <c r="C126" s="9" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="8"/>
       <c r="B127" s="8"/>
       <c r="C127" s="9" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="8"/>
       <c r="B128" s="8"/>
       <c r="C128" s="9" t="s">
@@ -3762,299 +3775,302 @@
     <row r="135" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="8"/>
       <c r="B135" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="C135" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="C135" s="9" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="8"/>
       <c r="B137" s="8"/>
       <c r="C137" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="8"/>
       <c r="B139" s="8"/>
       <c r="C139" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="8"/>
       <c r="B140" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C140" s="9" t="s">
         <v>298</v>
-      </c>
-      <c r="C140" s="9" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="8"/>
       <c r="B141" s="8"/>
       <c r="C141" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="8" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="8" t="s">
+      <c r="B145" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="B145" s="8" t="s">
+      <c r="C145" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="C145" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D145" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="8"/>
       <c r="B147" s="8"/>
       <c r="C147" s="9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="9" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="8"/>
       <c r="B150" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C150" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="C150" s="9" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="8"/>
       <c r="B151" s="8"/>
       <c r="C151" s="9" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="8"/>
       <c r="B152" s="8"/>
       <c r="C152" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="8"/>
       <c r="B153" s="8"/>
       <c r="C153" s="9" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="8"/>
       <c r="B155" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C155" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C155" s="9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="8"/>
       <c r="B158" s="8"/>
       <c r="C158" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="8"/>
       <c r="B159" s="8"/>
       <c r="C159" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="8"/>
       <c r="B160" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C160" s="9" t="s">
         <v>323</v>
-      </c>
-      <c r="C160" s="9" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="8"/>
       <c r="B161" s="8"/>
       <c r="C161" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="8"/>
       <c r="B163" s="8"/>
       <c r="C163" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="8"/>
       <c r="B164" s="8"/>
       <c r="C164" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="8"/>
       <c r="B165" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C165" s="9" t="s">
         <v>329</v>
-      </c>
-      <c r="C165" s="9" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="8"/>
       <c r="B166" s="8"/>
       <c r="C166" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="8"/>
       <c r="B167" s="8"/>
       <c r="C167" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="8"/>
       <c r="B168" s="8"/>
       <c r="C168" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="8"/>
       <c r="B169" s="8"/>
       <c r="C169" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="8"/>
       <c r="B170" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C170" s="9" t="s">
         <v>335</v>
-      </c>
-      <c r="C170" s="9" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="8"/>
       <c r="B171" s="8"/>
       <c r="C171" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A172" s="8"/>
       <c r="B172" s="8"/>
       <c r="C172" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="8"/>
       <c r="B173" s="8"/>
       <c r="C173" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A174" s="8"/>
       <c r="B174" s="8"/>
       <c r="C174" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
@@ -4062,223 +4078,223 @@
         <v>269</v>
       </c>
       <c r="B175" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C175" s="9" t="s">
         <v>341</v>
-      </c>
-      <c r="C175" s="9" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A176" s="8"/>
       <c r="B176" s="8"/>
       <c r="C176" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A177" s="8"/>
       <c r="B177" s="8"/>
       <c r="C177" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="C178" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A179" s="8"/>
       <c r="B179" s="8"/>
       <c r="C179" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A180" s="8"/>
       <c r="B180" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C180" s="9" t="s">
         <v>347</v>
-      </c>
-      <c r="C180" s="9" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="8"/>
       <c r="B181" s="8"/>
       <c r="C181" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="C182" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="C183" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="C184" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A185" s="8"/>
       <c r="B185" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="C185" s="9" t="s">
         <v>353</v>
-      </c>
-      <c r="C185" s="9" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="C186" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="C187" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="C188" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
       <c r="C189" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="8"/>
       <c r="B190" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C190" s="9" t="s">
         <v>359</v>
-      </c>
-      <c r="C190" s="9" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="8"/>
       <c r="B191" s="8"/>
       <c r="C191" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A192" s="8"/>
       <c r="B192" s="8"/>
       <c r="C192" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
       <c r="C193" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="C194" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A195" s="8"/>
       <c r="B195" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C195" s="9" t="s">
         <v>365</v>
-      </c>
-      <c r="C195" s="9" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
       <c r="C196" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A197" s="8"/>
       <c r="B197" s="8"/>
       <c r="C197" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A198" s="8"/>
       <c r="B198" s="8"/>
       <c r="C198" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
       <c r="C199" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A200" s="8"/>
       <c r="B200" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C200" s="9" t="s">
         <v>371</v>
-      </c>
-      <c r="C200" s="9" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A201" s="8"/>
       <c r="B201" s="8"/>
       <c r="C201" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
       <c r="C202" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A203" s="8"/>
       <c r="B203" s="8"/>
       <c r="C203" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A204" s="8"/>
       <c r="B204" s="8"/>
       <c r="C204" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>